<commit_message>
string generator fixed, fourbyfour tested function
</commit_message>
<xml_diff>
--- a/16by16_index.xlsx
+++ b/16by16_index.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -630,7 +630,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5">
-        <f t="shared" ref="A5:A20" si="25">A4+16</f>
+        <f t="shared" ref="A5:A16" si="25">A4+16</f>
         <v>65</v>
       </c>
       <c r="B5">
@@ -700,63 +700,63 @@
         <v>81</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B20" si="26">B5+16</f>
+        <f t="shared" ref="B6:B16" si="26">B5+16</f>
         <v>82</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C20" si="27">C5+16</f>
+        <f t="shared" ref="C6:C16" si="27">C5+16</f>
         <v>83</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D20" si="28">D5+16</f>
+        <f t="shared" ref="D6:D16" si="28">D5+16</f>
         <v>84</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E20" si="29">E5+16</f>
+        <f t="shared" ref="E6:E16" si="29">E5+16</f>
         <v>85</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F20" si="30">F5+16</f>
+        <f t="shared" ref="F6:F16" si="30">F5+16</f>
         <v>86</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G20" si="31">G5+16</f>
+        <f t="shared" ref="G6:G16" si="31">G5+16</f>
         <v>87</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H20" si="32">H5+16</f>
+        <f t="shared" ref="H6:H16" si="32">H5+16</f>
         <v>88</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I20" si="33">I5+16</f>
+        <f t="shared" ref="I6:I16" si="33">I5+16</f>
         <v>89</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J20" si="34">J5+16</f>
+        <f t="shared" ref="J6:J16" si="34">J5+16</f>
         <v>90</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K20" si="35">K5+16</f>
+        <f t="shared" ref="K6:K16" si="35">K5+16</f>
         <v>91</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L6:L20" si="36">L5+16</f>
+        <f t="shared" ref="L6:L16" si="36">L5+16</f>
         <v>92</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M20" si="37">M5+16</f>
+        <f t="shared" ref="M6:M16" si="37">M5+16</f>
         <v>93</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:N20" si="38">N5+16</f>
+        <f t="shared" ref="N6:N16" si="38">N5+16</f>
         <v>94</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O20" si="39">O5+16</f>
+        <f t="shared" ref="O6:O16" si="39">O5+16</f>
         <v>95</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:P20" si="40">P5+16</f>
+        <f t="shared" ref="P6:P16" si="40">P5+16</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sixteenby sixteen edge detection successful, modelsim simulation finish, Done
</commit_message>
<xml_diff>
--- a/16by16_index.xlsx
+++ b/16by16_index.xlsx
@@ -31,12 +31,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -51,8 +57,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -360,7 +367,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -653,19 +660,19 @@
         <f t="shared" si="14"/>
         <v>70</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="15"/>
         <v>71</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <f t="shared" si="16"/>
         <v>72</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <f t="shared" si="17"/>
         <v>73</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <f t="shared" si="18"/>
         <v>74</v>
       </c>
@@ -719,19 +726,19 @@
         <f t="shared" ref="F6:F16" si="30">F5+16</f>
         <v>86</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <f t="shared" ref="G6:G16" si="31">G5+16</f>
         <v>87</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <f t="shared" ref="H6:H16" si="32">H5+16</f>
         <v>88</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <f t="shared" ref="I6:I16" si="33">I5+16</f>
         <v>89</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <f t="shared" ref="J6:J16" si="34">J5+16</f>
         <v>90</v>
       </c>
@@ -785,19 +792,19 @@
         <f t="shared" si="30"/>
         <v>102</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f t="shared" si="31"/>
         <v>103</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <f t="shared" si="32"/>
         <v>104</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <f t="shared" si="33"/>
         <v>105</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <f t="shared" si="34"/>
         <v>106</v>
       </c>
@@ -851,19 +858,19 @@
         <f t="shared" si="30"/>
         <v>118</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" si="31"/>
         <v>119</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <f t="shared" si="32"/>
         <v>120</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <f t="shared" si="33"/>
         <v>121</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <f t="shared" si="34"/>
         <v>122</v>
       </c>
@@ -917,19 +924,19 @@
         <f t="shared" si="30"/>
         <v>134</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="31"/>
         <v>135</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <f t="shared" si="32"/>
         <v>136</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <f t="shared" si="33"/>
         <v>137</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <f t="shared" si="34"/>
         <v>138</v>
       </c>

</xml_diff>